<commit_message>
Setup info file for 8 rings.
</commit_message>
<xml_diff>
--- a/MosaicReconstruction/example/param_files/Cerebellum_8Rings.xlsx
+++ b/MosaicReconstruction/example/param_files/Cerebellum_8Rings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t xml:space="preserve">sample_name</t>
   </si>
@@ -37,10 +37,28 @@
     <t xml:space="preserve">ring</t>
   </si>
   <si>
-    <t xml:space="preserve">CerebellumLocal_0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">065_GMB_localScans_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
+    <t xml:space="preserve">cerebellum_8rings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">064_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">065_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">066_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">067_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">068_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">069_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">070_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
   </si>
 </sst>
 </file>
@@ -149,10 +167,10 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="71.87"/>
@@ -202,29 +220,123 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D3" s="1"/>
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D4" s="1"/>
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D5" s="1"/>
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C10" s="1"/>

</xml_diff>

<commit_message>
Correct wrong scan numbers in info file.
</commit_message>
<xml_diff>
--- a/MosaicReconstruction/example/param_files/Cerebellum_8Rings.xlsx
+++ b/MosaicReconstruction/example/param_files/Cerebellum_8Rings.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
   <si>
     <t xml:space="preserve">sample_name</t>
   </si>
@@ -41,24 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">064_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">065_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">066_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">067_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">068_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">069_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
-  </si>
-  <si>
-    <t xml:space="preserve">070_GMB_ringscan_500mA_Cu100_gap5p7_orca_10x_dist50mm_100ms</t>
   </si>
 </sst>
 </file>
@@ -167,10 +149,10 @@
   <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="71.87"/>
@@ -241,7 +223,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -258,7 +240,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
@@ -275,7 +257,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -292,7 +274,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -309,7 +291,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
@@ -326,7 +308,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>

</xml_diff>